<commit_message>
Changed the duration marker
</commit_message>
<xml_diff>
--- a/scheduler.xlsx
+++ b/scheduler.xlsx
@@ -598,17 +598,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -682,17 +682,17 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -766,37 +766,37 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
@@ -870,52 +870,52 @@
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr"/>
@@ -989,27 +989,27 @@
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr"/>
@@ -1083,52 +1083,52 @@
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr"/>
@@ -1202,52 +1202,52 @@
       <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AO8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AP8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AQ8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AR8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AS8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AT8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AU8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AV8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AW8" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AX8" t="inlineStr"/>
@@ -1321,27 +1321,27 @@
       <c r="AW9" t="inlineStr"/>
       <c r="AX9" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AY9" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="AZ9" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="BA9" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="BB9" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="BC9" t="inlineStr"/>
@@ -1415,7 +1415,7 @@
       <c r="BB10" t="inlineStr"/>
       <c r="BC10" t="inlineStr">
         <is>
-          <t>^</t>
+          <t>^====</t>
         </is>
       </c>
       <c r="BD10" t="inlineStr"/>

</xml_diff>